<commit_message>
Minor update/clarification notes to data curation dictionary
</commit_message>
<xml_diff>
--- a/UNITE_curation_dictionary.xlsx
+++ b/UNITE_curation_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ari/Dropbox/Documents/UDA/PROJECTS- ICU big data/UNITE COVID/UNITE-COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6218D79F-8DA6-7F48-9D75-2F632F90227F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465EFCF4-E043-5A40-A566-70442CAD5F2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="3080" windowWidth="39020" windowHeight="24600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="426">
   <si>
     <t>variable number</t>
   </si>
@@ -1287,6 +1287,18 @@
   </si>
   <si>
     <t>missing likely to represent not given</t>
+  </si>
+  <si>
+    <t>There are a number of patients with implausible weights &lt; 40kg</t>
+  </si>
+  <si>
+    <t>Represents the daily dose of all antiplatelets on day 1</t>
+  </si>
+  <si>
+    <t>Dose of t/p LMWH on first day of ICU admission</t>
+  </si>
+  <si>
+    <t>Represents the daily dose of LMWH on first day of ICU admission (irrespective of whether therapeutic or prophylactic)</t>
   </si>
 </sst>
 </file>
@@ -1678,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="I200" sqref="I200"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2198,7 +2210,9 @@
       <c r="H11" s="5">
         <v>268</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>422</v>
+      </c>
       <c r="J11" s="5" t="s">
         <v>51</v>
       </c>
@@ -7516,7 +7530,9 @@
       <c r="D137" s="20" t="s">
         <v>379</v>
       </c>
-      <c r="E137" s="6"/>
+      <c r="E137" s="6" t="s">
+        <v>424</v>
+      </c>
       <c r="F137" s="20" t="s">
         <v>376</v>
       </c>
@@ -10138,7 +10154,9 @@
       <c r="D193" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="E193" s="24"/>
+      <c r="E193" s="24" t="s">
+        <v>425</v>
+      </c>
       <c r="F193" s="24" t="s">
         <v>178</v>
       </c>
@@ -10182,7 +10200,9 @@
       <c r="D194" s="24" t="s">
         <v>420</v>
       </c>
-      <c r="E194" s="24"/>
+      <c r="E194" s="24" t="s">
+        <v>423</v>
+      </c>
       <c r="F194" s="24" t="s">
         <v>178</v>
       </c>

</xml_diff>

<commit_message>
Minor update to 2.2.1
</commit_message>
<xml_diff>
--- a/UNITE_curation_dictionary.xlsx
+++ b/UNITE_curation_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ari/Dropbox/Documents/UDA/PROJECTS- ICU big data/UNITE COVID/UNITE-COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DADC07-11EE-BB46-AEAC-35B7C412903C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB3924F-F495-C44F-B210-48CFCADE4810}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="1400" windowWidth="39020" windowHeight="24600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2900" windowWidth="39020" windowHeight="24600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="518">
   <si>
     <t>variable number</t>
   </si>
@@ -808,9 +808,6 @@
     <t>antibiotic names</t>
   </si>
   <si>
-    <t>don't know what the following numbers are: 0, 1, 3, 10, 45,56,67,69</t>
-  </si>
-  <si>
     <t>INF_ANTIFUNG_YN</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
   </si>
   <si>
     <t>Name of antifungal administered</t>
-  </si>
-  <si>
-    <t>missing antifungal codes</t>
   </si>
   <si>
     <t>INF_ANTIFUNG2_INT</t>
@@ -1578,6 +1572,9 @@
   </si>
   <si>
     <t>Fibrinogen at ICU admission</t>
+  </si>
+  <si>
+    <t>Some invalid codes recoded to NA</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1654,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1676,34 +1673,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1774,11 +1750,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1997,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2487,7 +2463,7 @@
         <v>268</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>50</v>
@@ -2521,10 +2497,10 @@
         <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>18</v>
@@ -2534,7 +2510,7 @@
         <v>4995</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>27</v>
@@ -2568,10 +2544,10 @@
         <v>53</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>18</v>
@@ -2611,7 +2587,7 @@
         <v>54</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="19" t="s">
@@ -2652,7 +2628,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="19" t="s">
@@ -2663,10 +2639,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -2697,7 +2673,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="19" t="s">
@@ -2709,7 +2685,7 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -2740,7 +2716,7 @@
         <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="19" t="s">
@@ -2751,10 +2727,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -2785,7 +2761,7 @@
         <v>58</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="19" t="s">
@@ -2826,10 +2802,10 @@
         <v>59</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>338</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>340</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>18</v>
@@ -2869,7 +2845,7 @@
         <v>60</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="19" t="s">
@@ -2910,7 +2886,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="19" t="s">
@@ -2951,7 +2927,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="19" t="s">
@@ -2992,7 +2968,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="19" t="s">
@@ -3033,14 +3009,14 @@
         <v>64</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H24" s="5">
         <v>158</v>
@@ -3076,7 +3052,7 @@
         <v>65</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="19" t="s">
@@ -3117,10 +3093,10 @@
         <v>66</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>18</v>
@@ -3160,10 +3136,10 @@
         <v>67</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F27" s="19" t="s">
         <v>18</v>
@@ -3203,10 +3179,10 @@
         <v>68</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>18</v>
@@ -3246,10 +3222,10 @@
         <v>69</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>18</v>
@@ -3289,7 +3265,7 @@
         <v>70</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="19" t="s">
@@ -3330,7 +3306,7 @@
         <v>71</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="19" t="s">
@@ -3371,7 +3347,7 @@
         <v>72</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="19" t="s">
@@ -3412,7 +3388,7 @@
         <v>73</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="19" t="s">
@@ -3453,14 +3429,14 @@
         <v>75</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H34" s="9">
         <v>171</v>
@@ -3496,16 +3472,16 @@
         <v>76</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3537,7 +3513,7 @@
         <v>77</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="25" t="s">
@@ -3578,7 +3554,7 @@
         <v>78</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="25" t="s">
@@ -3619,7 +3595,7 @@
         <v>79</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="25" t="s">
@@ -3660,7 +3636,7 @@
         <v>80</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="25" t="s">
@@ -3701,7 +3677,7 @@
         <v>81</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="25" t="s">
@@ -3715,7 +3691,7 @@
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
@@ -3746,16 +3722,16 @@
         <v>82</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H41" s="9">
         <v>1675</v>
@@ -3791,7 +3767,7 @@
         <v>83</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
@@ -3871,7 +3847,7 @@
         <v>85</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9" t="s">
@@ -3910,7 +3886,7 @@
         <v>86</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9" t="s">
@@ -3949,7 +3925,7 @@
         <v>87</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9" t="s">
@@ -3988,7 +3964,7 @@
         <v>88</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9" t="s">
@@ -4027,7 +4003,7 @@
         <v>89</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9" t="s">
@@ -4066,7 +4042,7 @@
         <v>90</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
@@ -4105,7 +4081,7 @@
         <v>91</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9" t="s">
@@ -4144,10 +4120,10 @@
         <v>92</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>177</v>
@@ -4185,7 +4161,7 @@
         <v>93</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9" t="s">
@@ -4224,7 +4200,7 @@
         <v>94</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9" t="s">
@@ -4263,7 +4239,7 @@
         <v>95</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9" t="s">
@@ -4291,7 +4267,7 @@
       <c r="Z54" s="9"/>
       <c r="AA54" s="9"/>
     </row>
-    <row r="55" spans="1:27" ht="12.75" customHeight="1" thickBot="1">
+    <row r="55" spans="1:27" ht="12.75" customHeight="1">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -4302,7 +4278,7 @@
         <v>96</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9" t="s">
@@ -4330,7 +4306,7 @@
       <c r="Z55" s="9"/>
       <c r="AA55" s="9"/>
     </row>
-    <row r="56" spans="1:27" ht="12.75" customHeight="1" thickBot="1">
+    <row r="56" spans="1:27" ht="12.75" customHeight="1">
       <c r="A56" s="8">
         <v>55</v>
       </c>
@@ -4340,8 +4316,8 @@
       <c r="C56" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="27" t="s">
-        <v>499</v>
+      <c r="D56" s="9" t="s">
+        <v>497</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="25" t="s">
@@ -4355,7 +4331,7 @@
       </c>
       <c r="I56" s="9"/>
       <c r="J56" s="9" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
@@ -4386,7 +4362,7 @@
         <v>98</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="25" t="s">
@@ -4400,7 +4376,7 @@
       </c>
       <c r="I57" s="9"/>
       <c r="J57" s="9" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -4431,7 +4407,7 @@
         <v>99</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="25" t="s">
@@ -4445,7 +4421,7 @@
       </c>
       <c r="I58" s="9"/>
       <c r="J58" s="9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -4476,7 +4452,7 @@
         <v>100</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="25" t="s">
@@ -4490,7 +4466,7 @@
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
@@ -4521,7 +4497,7 @@
         <v>101</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="25" t="s">
@@ -4535,7 +4511,7 @@
       </c>
       <c r="I60" s="9"/>
       <c r="J60" s="9" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -4566,7 +4542,7 @@
         <v>102</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="25" t="s">
@@ -4580,7 +4556,7 @@
       </c>
       <c r="I61" s="9"/>
       <c r="J61" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
@@ -4611,7 +4587,7 @@
         <v>103</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="25" t="s">
@@ -4625,7 +4601,7 @@
       </c>
       <c r="I62" s="9"/>
       <c r="J62" s="9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
@@ -4656,7 +4632,7 @@
         <v>104</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="25" t="s">
@@ -4670,7 +4646,7 @@
       </c>
       <c r="I63" s="9"/>
       <c r="J63" s="9" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
@@ -4701,7 +4677,7 @@
         <v>105</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="25" t="s">
@@ -4715,7 +4691,7 @@
       </c>
       <c r="I64" s="9"/>
       <c r="J64" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
@@ -4746,7 +4722,7 @@
         <v>106</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="25" t="s">
@@ -4760,7 +4736,7 @@
       </c>
       <c r="I65" s="9"/>
       <c r="J65" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
@@ -5252,7 +5228,7 @@
         <v>25</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H76" s="4">
         <v>2545</v>
@@ -6262,7 +6238,7 @@
         <v>195</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E99" s="25"/>
       <c r="F99" s="25" t="s">
@@ -6305,7 +6281,7 @@
         <v>196</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E100" s="25"/>
       <c r="F100" s="25" t="s">
@@ -6348,7 +6324,7 @@
         <v>197</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E101" s="25"/>
       <c r="F101" s="26"/>
@@ -6382,7 +6358,7 @@
         <v>198</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E102" s="25"/>
       <c r="F102" s="25" t="s">
@@ -6396,7 +6372,7 @@
       </c>
       <c r="I102" s="9"/>
       <c r="J102" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
@@ -6427,7 +6403,7 @@
         <v>199</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E103" s="25"/>
       <c r="F103" s="25"/>
@@ -6464,7 +6440,7 @@
         <v>200</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E104" s="25"/>
       <c r="F104" s="25" t="s">
@@ -6478,7 +6454,7 @@
       </c>
       <c r="I104" s="9"/>
       <c r="J104" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K104" s="9"/>
       <c r="L104" s="9"/>
@@ -6509,7 +6485,7 @@
         <v>201</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E105" s="25"/>
       <c r="F105" s="25"/>
@@ -6546,7 +6522,7 @@
         <v>202</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E106" s="25"/>
       <c r="F106" s="25" t="s">
@@ -6560,7 +6536,7 @@
       </c>
       <c r="I106" s="9"/>
       <c r="J106" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K106" s="9"/>
       <c r="L106" s="9"/>
@@ -6591,7 +6567,7 @@
         <v>203</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E107" s="25"/>
       <c r="F107" s="25"/>
@@ -6628,7 +6604,7 @@
         <v>204</v>
       </c>
       <c r="D108" s="25" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E108" s="25"/>
       <c r="F108" s="25" t="s">
@@ -6642,7 +6618,7 @@
       </c>
       <c r="I108" s="9"/>
       <c r="J108" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="K108" s="9"/>
       <c r="L108" s="9"/>
@@ -6673,7 +6649,7 @@
         <v>205</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E109" s="25"/>
       <c r="F109" s="25"/>
@@ -6710,7 +6686,7 @@
         <v>206</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E110" s="25"/>
       <c r="F110" s="25" t="s">
@@ -6724,7 +6700,7 @@
       </c>
       <c r="I110" s="9"/>
       <c r="J110" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="K110" s="9"/>
       <c r="L110" s="9"/>
@@ -6755,7 +6731,7 @@
         <v>207</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E111" s="25"/>
       <c r="F111" s="25"/>
@@ -6794,7 +6770,7 @@
         <v>208</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E112" s="25"/>
       <c r="F112" s="25"/>
@@ -6804,7 +6780,7 @@
       </c>
       <c r="I112" s="9"/>
       <c r="J112" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K112" s="9"/>
       <c r="L112" s="9"/>
@@ -6835,7 +6811,7 @@
         <v>209</v>
       </c>
       <c r="D113" s="25" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E113" s="25"/>
       <c r="F113" s="25" t="s">
@@ -6878,7 +6854,7 @@
         <v>210</v>
       </c>
       <c r="D114" s="25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E114" s="25"/>
       <c r="G114" s="25"/>
@@ -6914,14 +6890,14 @@
         <v>211</v>
       </c>
       <c r="D115" s="25" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E115" s="25"/>
       <c r="F115" s="25" t="s">
         <v>18</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H115" s="9"/>
       <c r="I115" s="9"/>
@@ -6955,14 +6931,14 @@
         <v>212</v>
       </c>
       <c r="D116" s="25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E116" s="25"/>
       <c r="F116" s="25" t="s">
         <v>18</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H116" s="9"/>
       <c r="I116" s="9"/>
@@ -6996,14 +6972,14 @@
         <v>213</v>
       </c>
       <c r="D117" s="25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E117" s="25"/>
       <c r="F117" s="25" t="s">
         <v>18</v>
       </c>
       <c r="G117" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H117" s="9"/>
       <c r="I117" s="9"/>
@@ -7037,14 +7013,14 @@
         <v>214</v>
       </c>
       <c r="D118" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E118" s="25"/>
       <c r="F118" s="25" t="s">
         <v>18</v>
       </c>
       <c r="G118" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H118" s="9"/>
       <c r="I118" s="9"/>
@@ -7078,14 +7054,14 @@
         <v>215</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E119" s="25"/>
       <c r="F119" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G119" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H119" s="9">
         <v>993</v>
@@ -7121,7 +7097,7 @@
         <v>216</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E120" s="25"/>
       <c r="F120" s="25" t="s">
@@ -7160,7 +7136,7 @@
         <v>217</v>
       </c>
       <c r="D121" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E121" s="25"/>
       <c r="F121" s="25" t="s">
@@ -7199,17 +7175,17 @@
         <v>218</v>
       </c>
       <c r="D122" s="25" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E122" s="25"/>
       <c r="F122" s="25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G122" s="25"/>
       <c r="H122" s="9"/>
       <c r="I122" s="9"/>
       <c r="J122" s="9" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K122" s="9"/>
       <c r="L122" s="9"/>
@@ -7240,7 +7216,7 @@
         <v>219</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E123" s="25"/>
       <c r="F123" s="25" t="s">
@@ -7250,7 +7226,7 @@
       <c r="H123" s="9"/>
       <c r="I123" s="9"/>
       <c r="J123" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K123" s="9"/>
       <c r="L123" s="9"/>
@@ -7281,7 +7257,7 @@
         <v>220</v>
       </c>
       <c r="D124" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E124" s="25"/>
       <c r="F124" s="25" t="s">
@@ -7291,7 +7267,7 @@
       <c r="H124" s="9"/>
       <c r="I124" s="9"/>
       <c r="J124" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K124" s="9"/>
       <c r="L124" s="9"/>
@@ -7322,7 +7298,7 @@
         <v>221</v>
       </c>
       <c r="D125" s="25" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E125" s="25"/>
       <c r="F125" s="25" t="s">
@@ -7361,7 +7337,7 @@
         <v>222</v>
       </c>
       <c r="D126" s="25" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E126" s="25"/>
       <c r="F126" s="25" t="s">
@@ -7404,14 +7380,14 @@
         <v>223</v>
       </c>
       <c r="D127" s="25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E127" s="25"/>
       <c r="F127" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G127" s="25" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H127" s="9">
         <v>1543</v>
@@ -7447,7 +7423,7 @@
         <v>224</v>
       </c>
       <c r="D128" s="25" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E128" s="25"/>
       <c r="F128" s="25" t="s">
@@ -7460,10 +7436,10 @@
         <v>1544</v>
       </c>
       <c r="I128" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J128" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K128" s="9"/>
       <c r="L128" s="9"/>
@@ -7494,10 +7470,10 @@
         <v>225</v>
       </c>
       <c r="D129" s="25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F129" s="9" t="s">
         <v>177</v>
@@ -7535,7 +7511,7 @@
         <v>226</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="11" t="s">
@@ -7576,7 +7552,7 @@
         <v>227</v>
       </c>
       <c r="D131" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="11" t="s">
@@ -7587,7 +7563,7 @@
         <v>251</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J131" s="5"/>
       <c r="K131" s="5"/>
@@ -7619,7 +7595,7 @@
         <v>228</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="11" t="s">
@@ -7630,7 +7606,7 @@
         <v>257</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J132" s="5"/>
       <c r="K132" s="5"/>
@@ -7662,7 +7638,7 @@
         <v>229</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="11" t="s">
@@ -7673,7 +7649,7 @@
         <v>1413</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J133" s="5"/>
       <c r="K133" s="5"/>
@@ -7705,7 +7681,7 @@
         <v>230</v>
       </c>
       <c r="D134" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="11" t="s">
@@ -7716,7 +7692,7 @@
         <v>1413</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J134" s="5"/>
       <c r="K134" s="5"/>
@@ -7748,7 +7724,7 @@
         <v>231</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="11" t="s">
@@ -7759,7 +7735,7 @@
         <v>1363</v>
       </c>
       <c r="I135" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J135" s="5"/>
       <c r="K135" s="5"/>
@@ -7791,14 +7767,14 @@
         <v>232</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H136" s="5">
         <v>208</v>
@@ -7834,18 +7810,18 @@
         <v>233</v>
       </c>
       <c r="D137" s="19" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F137" s="19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
       <c r="I137" s="19" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J137" s="5"/>
       <c r="K137" s="5"/>
@@ -7877,14 +7853,14 @@
         <v>234</v>
       </c>
       <c r="D138" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H138" s="5">
         <v>208</v>
@@ -7920,16 +7896,16 @@
         <v>235</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
       <c r="I139" s="19" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J139" s="5"/>
       <c r="K139" s="5"/>
@@ -7996,22 +7972,22 @@
         <v>237</v>
       </c>
       <c r="D141" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E141" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F141" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G141" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H141" s="5">
         <v>0</v>
       </c>
       <c r="I141" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J141" s="5"/>
       <c r="K141" s="5"/>
@@ -8043,22 +8019,22 @@
         <v>238</v>
       </c>
       <c r="D142" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="E142" s="19" t="s">
         <v>383</v>
-      </c>
-      <c r="E142" s="19" t="s">
-        <v>385</v>
       </c>
       <c r="F142" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G142" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H142" s="11">
         <v>0</v>
       </c>
       <c r="I142" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J142" s="5"/>
       <c r="K142" s="5"/>
@@ -8090,22 +8066,22 @@
         <v>239</v>
       </c>
       <c r="D143" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E143" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F143" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G143" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H143" s="11">
         <v>0</v>
       </c>
       <c r="I143" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J143" s="5"/>
       <c r="K143" s="5"/>
@@ -8137,22 +8113,22 @@
         <v>240</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E144" s="19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F144" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G144" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H144" s="11">
         <v>0</v>
       </c>
       <c r="I144" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J144" s="5"/>
       <c r="K144" s="5"/>
@@ -8184,22 +8160,22 @@
         <v>241</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E145" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F145" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G145" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H145" s="11">
         <v>0</v>
       </c>
       <c r="I145" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J145" s="5"/>
       <c r="K145" s="5"/>
@@ -8231,22 +8207,22 @@
         <v>242</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E146" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F146" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G146" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H146" s="11">
         <v>0</v>
       </c>
       <c r="I146" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J146" s="5"/>
       <c r="K146" s="5"/>
@@ -8278,7 +8254,7 @@
         <v>243</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E147" s="5"/>
       <c r="F147" s="19" t="s">
@@ -8289,7 +8265,7 @@
         <v>687</v>
       </c>
       <c r="I147" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J147" s="5"/>
       <c r="K147" s="5"/>
@@ -8321,22 +8297,22 @@
         <v>244</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E148" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F148" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G148" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H148" s="5">
         <v>0</v>
       </c>
       <c r="I148" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J148" s="5"/>
       <c r="K148" s="5"/>
@@ -8368,22 +8344,22 @@
         <v>245</v>
       </c>
       <c r="D149" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="E149" s="19" t="s">
         <v>392</v>
-      </c>
-      <c r="E149" s="19" t="s">
-        <v>394</v>
       </c>
       <c r="F149" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G149" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H149" s="5">
         <v>0</v>
       </c>
       <c r="I149" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J149" s="5"/>
       <c r="K149" s="5"/>
@@ -8415,22 +8391,22 @@
         <v>246</v>
       </c>
       <c r="D150" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E150" s="19" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F150" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G150" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H150" s="5">
         <v>0</v>
       </c>
       <c r="I150" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J150" s="5"/>
       <c r="K150" s="5"/>
@@ -8462,22 +8438,22 @@
         <v>247</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E151" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F151" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G151" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H151" s="5">
         <v>0</v>
       </c>
       <c r="I151" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J151" s="5"/>
       <c r="K151" s="5"/>
@@ -8509,22 +8485,22 @@
         <v>248</v>
       </c>
       <c r="D152" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E152" s="19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F152" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G152" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H152" s="5">
         <v>0</v>
       </c>
       <c r="I152" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J152" s="5"/>
       <c r="K152" s="5"/>
@@ -8556,22 +8532,22 @@
         <v>249</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E153" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F153" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G153" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H153" s="11">
         <v>0</v>
       </c>
       <c r="I153" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J153" s="5"/>
       <c r="K153" s="5"/>
@@ -8603,7 +8579,7 @@
         <v>250</v>
       </c>
       <c r="D154" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E154" s="5"/>
       <c r="F154" s="19" t="s">
@@ -8646,20 +8622,20 @@
         <v>251</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E155" s="5"/>
       <c r="F155" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G155" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H155" s="5">
         <v>2911</v>
       </c>
       <c r="I155" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J155" s="5"/>
       <c r="K155" s="5"/>
@@ -8691,18 +8667,18 @@
         <v>252</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E156" s="5"/>
       <c r="F156" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G156" s="5"/>
       <c r="H156" s="5">
         <v>2918</v>
       </c>
       <c r="I156" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J156" s="5"/>
       <c r="K156" s="5"/>
@@ -8734,20 +8710,20 @@
         <v>253</v>
       </c>
       <c r="D157" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E157" s="5"/>
       <c r="F157" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H157" s="5">
         <v>2949</v>
       </c>
       <c r="I157" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J157" s="5"/>
       <c r="K157" s="5"/>
@@ -8779,7 +8755,7 @@
         <v>254</v>
       </c>
       <c r="D158" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E158" s="5"/>
       <c r="F158" s="19" t="s">
@@ -8822,20 +8798,18 @@
         <v>255</v>
       </c>
       <c r="D159" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>260</v>
       </c>
       <c r="F159" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G159" s="5"/>
-      <c r="H159" s="5">
-        <v>795</v>
-      </c>
+      <c r="H159" s="5"/>
       <c r="I159" s="11" t="s">
-        <v>262</v>
+        <v>517</v>
       </c>
       <c r="J159" s="5"/>
       <c r="K159" s="5"/>
@@ -8867,20 +8841,18 @@
         <v>256</v>
       </c>
       <c r="D160" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E160" s="11" t="s">
         <v>260</v>
       </c>
       <c r="F160" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G160" s="5"/>
-      <c r="H160" s="5">
-        <v>4285</v>
-      </c>
-      <c r="I160" s="5" t="s">
-        <v>262</v>
+      <c r="H160" s="5"/>
+      <c r="I160" s="11" t="s">
+        <v>517</v>
       </c>
       <c r="J160" s="5"/>
       <c r="K160" s="5"/>
@@ -8912,20 +8884,18 @@
         <v>257</v>
       </c>
       <c r="D161" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>260</v>
       </c>
       <c r="F161" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G161" s="5"/>
-      <c r="H161" s="5">
-        <v>2335</v>
-      </c>
+      <c r="H161" s="5"/>
       <c r="I161" s="11" t="s">
-        <v>262</v>
+        <v>517</v>
       </c>
       <c r="J161" s="5"/>
       <c r="K161" s="5"/>
@@ -8957,22 +8927,20 @@
         <v>259</v>
       </c>
       <c r="D162" s="22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E162" s="14" t="s">
         <v>260</v>
       </c>
       <c r="F162" s="22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G162" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="H162" s="15">
-        <v>4719</v>
-      </c>
-      <c r="I162" s="14" t="s">
-        <v>262</v>
+      <c r="H162" s="15"/>
+      <c r="I162" s="28" t="s">
+        <v>517</v>
       </c>
       <c r="J162" s="9"/>
       <c r="K162" s="9"/>
@@ -9001,10 +8969,10 @@
         <v>258</v>
       </c>
       <c r="C163" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="D163" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="D163" s="14" t="s">
-        <v>264</v>
       </c>
       <c r="E163" s="16"/>
       <c r="F163" s="14" t="s">
@@ -9013,10 +8981,10 @@
       <c r="G163" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H163" s="15">
-        <v>194</v>
-      </c>
-      <c r="I163" s="17"/>
+      <c r="H163" s="15"/>
+      <c r="I163" s="28" t="s">
+        <v>517</v>
+      </c>
       <c r="J163" s="9"/>
       <c r="K163" s="9"/>
       <c r="L163" s="9"/>
@@ -9044,21 +9012,19 @@
         <v>258</v>
       </c>
       <c r="C164" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D164" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D164" s="14" t="s">
+      <c r="E164" s="14" t="s">
         <v>266</v>
-      </c>
-      <c r="E164" s="14" t="s">
-        <v>267</v>
       </c>
       <c r="F164" s="17"/>
       <c r="G164" s="17"/>
-      <c r="H164" s="15">
-        <v>4733</v>
-      </c>
-      <c r="I164" s="14" t="s">
-        <v>268</v>
+      <c r="H164" s="15"/>
+      <c r="I164" s="28" t="s">
+        <v>517</v>
       </c>
       <c r="J164" s="9"/>
       <c r="K164" s="9"/>
@@ -9087,21 +9053,19 @@
         <v>258</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E165" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F165" s="17"/>
       <c r="G165" s="17"/>
-      <c r="H165" s="15">
-        <v>4957</v>
-      </c>
-      <c r="I165" s="14" t="s">
-        <v>268</v>
+      <c r="H165" s="15"/>
+      <c r="I165" s="28" t="s">
+        <v>517</v>
       </c>
       <c r="J165" s="9"/>
       <c r="K165" s="9"/>
@@ -9130,21 +9094,19 @@
         <v>258</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F166" s="17"/>
       <c r="G166" s="17"/>
-      <c r="H166" s="15">
-        <v>4989</v>
-      </c>
-      <c r="I166" s="14" t="s">
-        <v>268</v>
+      <c r="H166" s="15"/>
+      <c r="I166" s="28" t="s">
+        <v>517</v>
       </c>
       <c r="J166" s="9"/>
       <c r="K166" s="9"/>
@@ -9173,21 +9135,19 @@
         <v>258</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F167" s="17"/>
       <c r="G167" s="17"/>
-      <c r="H167" s="15">
-        <v>4992</v>
-      </c>
-      <c r="I167" s="14" t="s">
-        <v>268</v>
+      <c r="H167" s="15"/>
+      <c r="I167" s="28" t="s">
+        <v>517</v>
       </c>
       <c r="J167" s="9"/>
       <c r="K167" s="9"/>
@@ -9216,10 +9176,10 @@
         <v>258</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E168" s="17"/>
       <c r="F168" s="14" t="s">
@@ -9259,10 +9219,10 @@
         <v>258</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E169" s="17"/>
       <c r="F169" s="14" t="s">
@@ -9302,23 +9262,23 @@
         <v>258</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E170" s="17"/>
       <c r="F170" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G170" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H170" s="15">
         <v>2335</v>
       </c>
       <c r="I170" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J170" s="9"/>
       <c r="K170" s="9"/>
@@ -9347,10 +9307,10 @@
         <v>258</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E171" s="17"/>
       <c r="F171" s="14" t="s">
@@ -9390,10 +9350,10 @@
         <v>258</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E172" s="17"/>
       <c r="F172" s="14" t="s">
@@ -9433,10 +9393,10 @@
         <v>258</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E173" s="17"/>
       <c r="F173" s="14" t="s">
@@ -9476,10 +9436,10 @@
         <v>258</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E174" s="17"/>
       <c r="F174" s="14" t="s">
@@ -9519,10 +9479,10 @@
         <v>258</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E175" s="17"/>
       <c r="F175" s="14" t="s">
@@ -9562,10 +9522,10 @@
         <v>258</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E176" s="17"/>
       <c r="F176" s="14" t="s">
@@ -9605,10 +9565,10 @@
         <v>258</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E177" s="17"/>
       <c r="F177" s="14" t="s">
@@ -9648,10 +9608,10 @@
         <v>258</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E178" s="17"/>
       <c r="F178" s="14" t="s">
@@ -9691,10 +9651,10 @@
         <v>258</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E179" s="17"/>
       <c r="F179" s="14" t="s">
@@ -9707,7 +9667,7 @@
         <v>2084</v>
       </c>
       <c r="I179" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J179" s="9"/>
       <c r="K179" s="9"/>
@@ -9736,19 +9696,19 @@
         <v>258</v>
       </c>
       <c r="C180" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D180" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E180" s="14" t="s">
         <v>302</v>
-      </c>
-      <c r="D180" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="E180" s="14" t="s">
-        <v>304</v>
       </c>
       <c r="F180" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G180" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H180" s="15">
         <v>4328</v>
@@ -9781,10 +9741,10 @@
         <v>258</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E181" s="17"/>
       <c r="F181" s="14" t="s">
@@ -9795,7 +9755,7 @@
         <v>690</v>
       </c>
       <c r="I181" s="17" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="J181" s="9"/>
       <c r="K181" s="9"/>
@@ -9824,17 +9784,17 @@
         <v>258</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E182" s="17"/>
       <c r="F182" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G182" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H182" s="15">
         <v>266</v>
@@ -9867,14 +9827,14 @@
         <v>258</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E183" s="17"/>
       <c r="F183" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G183" s="17"/>
       <c r="H183" s="15">
@@ -9908,17 +9868,17 @@
         <v>258</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E184" s="17"/>
       <c r="F184" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G184" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H184" s="15">
         <v>436</v>
@@ -9951,14 +9911,14 @@
         <v>258</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E185" s="17"/>
       <c r="F185" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G185" s="17"/>
       <c r="H185" s="15">
@@ -9992,14 +9952,14 @@
         <v>258</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E186" s="17"/>
       <c r="F186" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G186" s="17"/>
       <c r="H186" s="15">
@@ -10033,23 +9993,23 @@
         <v>258</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D187" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E187" s="17"/>
       <c r="F187" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G187" s="28" t="s">
-        <v>512</v>
+      <c r="G187" s="27" t="s">
+        <v>510</v>
       </c>
       <c r="H187" s="15">
         <v>270</v>
       </c>
       <c r="I187" s="17" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J187" s="9"/>
       <c r="K187" s="9"/>
@@ -10078,14 +10038,14 @@
         <v>258</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E188" s="17"/>
       <c r="F188" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G188" s="17"/>
       <c r="H188" s="15">
@@ -10119,10 +10079,10 @@
         <v>258</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E189" s="17"/>
       <c r="F189" s="14" t="s">
@@ -10162,14 +10122,14 @@
         <v>258</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E190" s="17"/>
       <c r="F190" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G190" s="17"/>
       <c r="H190" s="15">
@@ -10203,10 +10163,10 @@
         <v>258</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E191" s="17"/>
       <c r="F191" s="14" t="s">
@@ -10246,10 +10206,10 @@
         <v>258</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E192" s="17"/>
       <c r="F192" s="14" t="s">
@@ -10262,7 +10222,7 @@
         <v>3394</v>
       </c>
       <c r="I192" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J192" s="9"/>
       <c r="K192" s="9"/>
@@ -10285,19 +10245,19 @@
     </row>
     <row r="193" spans="1:27" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="A193" s="23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B193" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D193" s="23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E193" s="23" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F193" s="23" t="s">
         <v>177</v>
@@ -10307,7 +10267,7 @@
         <v>682</v>
       </c>
       <c r="I193" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J193" s="23"/>
       <c r="K193" s="23"/>
@@ -10330,19 +10290,19 @@
     </row>
     <row r="194" spans="1:27" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="A194" s="23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B194" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C194" s="23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D194" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E194" s="23" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F194" s="23" t="s">
         <v>177</v>
@@ -10352,7 +10312,7 @@
         <v>3894</v>
       </c>
       <c r="I194" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J194" s="23"/>
       <c r="K194" s="23"/>

</xml_diff>